<commit_message>
Added 2nd diet plan
</commit_message>
<xml_diff>
--- a/DietPlan.xlsx
+++ b/DietPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sr.w/Documents/GitHub/fat-loss-plans/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1992E32-7E50-DF44-A962-2C19A06165E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BDE01C3-CC7A-E24A-9987-9793D909C983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="51200" windowHeight="26600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="51200" windowHeight="26600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="目标设定" sheetId="4" r:id="rId1"/>
@@ -813,6 +813,24 @@
     <xf numFmtId="166" fontId="8" fillId="5" borderId="5" xfId="5" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -849,43 +867,25 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="5" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="5" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="5" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="5" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="5" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3388,7 +3388,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView zoomScale="104" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3452,7 +3452,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="51" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -3500,7 +3500,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="25" t="s">
         <v>65</v>
       </c>
@@ -3546,47 +3546,48 @@
       </c>
     </row>
     <row r="4" spans="1:14" s="25" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="59" t="s">
+      <c r="A4" s="51"/>
+      <c r="B4" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="61">
+      <c r="C4" s="44"/>
+      <c r="D4" s="45">
         <v>10</v>
       </c>
-      <c r="E4" s="62">
+      <c r="E4" s="46">
         <v>21</v>
       </c>
-      <c r="F4" s="63" t="s">
+      <c r="F4" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="64">
+      <c r="G4" s="27">
+        <f t="shared" si="0"/>
         <v>150.78</v>
       </c>
-      <c r="H4" s="64">
+      <c r="H4" s="48">
         <v>2.94</v>
       </c>
-      <c r="I4" s="64">
+      <c r="I4" s="48">
         <v>1.68</v>
       </c>
-      <c r="J4" s="64">
+      <c r="J4" s="48">
         <v>15.92</v>
       </c>
-      <c r="K4" s="64">
+      <c r="K4" s="48">
         <v>7.18</v>
       </c>
-      <c r="L4" s="63">
+      <c r="L4" s="47">
         <v>0.14000000000000001</v>
       </c>
-      <c r="M4" s="63">
+      <c r="M4" s="47">
         <v>0.08</v>
       </c>
-      <c r="N4" s="63">
+      <c r="N4" s="47">
         <v>0.75800000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="25" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="25" t="s">
         <v>45</v>
       </c>
@@ -3630,7 +3631,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" s="20" customFormat="1" ht="52" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="53" t="s">
         <v>48</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -3663,7 +3664,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="47"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="20" t="s">
         <v>49</v>
       </c>
@@ -3692,7 +3693,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="47"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="20" t="s">
         <v>50</v>
       </c>
@@ -3721,7 +3722,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" s="20" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="47"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="20" t="s">
         <v>51</v>
       </c>
@@ -3752,7 +3753,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" s="20" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="47"/>
+      <c r="A10" s="53"/>
       <c r="B10" s="20" t="s">
         <v>87</v>
       </c>
@@ -3812,7 +3813,7 @@
       <c r="N11" s="18"/>
     </row>
     <row r="12" spans="1:14" s="28" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="55" t="s">
         <v>71</v>
       </c>
       <c r="B12" s="41" t="s">
@@ -3860,7 +3861,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" s="28" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
+      <c r="A13" s="56"/>
       <c r="B13" s="28" t="s">
         <v>59</v>
       </c>
@@ -3904,7 +3905,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" s="28" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
+      <c r="A14" s="57"/>
       <c r="B14" s="28" t="s">
         <v>74</v>
       </c>
@@ -3937,7 +3938,7 @@
       <c r="K14" s="30"/>
     </row>
     <row r="15" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="51" t="s">
         <v>61</v>
       </c>
       <c r="B15" s="25" t="s">
@@ -3985,7 +3986,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="25" t="s">
         <v>94</v>
       </c>
@@ -4031,7 +4032,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="25" t="s">
         <v>65</v>
       </c>
@@ -4077,7 +4078,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" s="22" customFormat="1" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="52" t="s">
         <v>48</v>
       </c>
       <c r="B18" s="22" t="s">
@@ -4122,7 +4123,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" s="22" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="46"/>
+      <c r="A19" s="52"/>
       <c r="B19" s="22" t="s">
         <v>46</v>
       </c>
@@ -4148,7 +4149,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" s="22" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
+      <c r="A20" s="52"/>
       <c r="B20" s="22" t="s">
         <v>79</v>
       </c>
@@ -4179,7 +4180,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" s="41" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="52" t="s">
+      <c r="A21" s="58" t="s">
         <v>71</v>
       </c>
       <c r="B21" s="28" t="s">
@@ -4227,7 +4228,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" s="41" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
+      <c r="A22" s="58"/>
       <c r="B22" s="41" t="s">
         <v>30</v>
       </c>
@@ -4270,7 +4271,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="51" t="s">
         <v>72</v>
       </c>
       <c r="B23" s="25" t="s">
@@ -4318,7 +4319,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="45"/>
+      <c r="A24" s="51"/>
       <c r="B24" s="25" t="s">
         <v>63</v>
       </c>
@@ -4364,7 +4365,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="45"/>
+      <c r="A25" s="51"/>
       <c r="B25" s="25" t="s">
         <v>105</v>
       </c>
@@ -4410,7 +4411,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="45"/>
+      <c r="A26" s="51"/>
       <c r="B26" s="25" t="s">
         <v>112</v>
       </c>
@@ -4456,7 +4457,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" s="22" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="52" t="s">
         <v>78</v>
       </c>
       <c r="B27" s="22" t="s">
@@ -4504,7 +4505,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="46"/>
+      <c r="A28" s="52"/>
       <c r="B28" s="22" t="s">
         <v>79</v>
       </c>
@@ -4521,7 +4522,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" s="22" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="46"/>
+      <c r="A29" s="52"/>
       <c r="B29" s="22" t="s">
         <v>82</v>
       </c>
@@ -4656,8 +4657,8 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="2"/>
-    <col min="2" max="2" width="13.6640625" style="44" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="44" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="50" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="50" customWidth="1"/>
     <col min="4" max="4" width="8.83203125" style="2"/>
     <col min="5" max="5" width="8.83203125" style="7"/>
     <col min="6" max="9" width="8.83203125" style="2"/>
@@ -4718,10 +4719,10 @@
       <c r="A2" s="3">
         <v>45807.209140721912</v>
       </c>
-      <c r="B2" s="43">
+      <c r="B2" s="49">
         <v>27</v>
       </c>
-      <c r="C2" s="43">
+      <c r="C2" s="49">
         <v>180</v>
       </c>
       <c r="D2" s="2">
@@ -6806,8 +6807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E56B043D-0020-F546-B9D9-4347F4985AEA}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6871,7 +6872,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="51" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -6919,7 +6920,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" s="25" customFormat="1" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="25" t="s">
         <v>32</v>
       </c>
@@ -6965,7 +6966,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" s="25" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="25" t="s">
         <v>45</v>
       </c>
@@ -7009,7 +7010,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" s="20" customFormat="1" ht="52" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="53" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="20" t="s">
@@ -7042,7 +7043,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="47"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="20" t="s">
         <v>49</v>
       </c>
@@ -7071,7 +7072,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="47"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="20" t="s">
         <v>50</v>
       </c>
@@ -7100,7 +7101,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" s="20" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="47"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="20" t="s">
         <v>51</v>
       </c>
@@ -7131,7 +7132,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" s="20" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="47"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="20" t="s">
         <v>87</v>
       </c>
@@ -7193,7 +7194,7 @@
       <c r="N10" s="18"/>
     </row>
     <row r="11" spans="1:14" s="28" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="54" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="28" t="s">
@@ -7239,7 +7240,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" s="28" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
+      <c r="A12" s="54"/>
       <c r="B12" s="28" t="s">
         <v>30</v>
       </c>
@@ -7285,7 +7286,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" s="28" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="48"/>
+      <c r="A13" s="54"/>
       <c r="B13" s="28" t="s">
         <v>59</v>
       </c>
@@ -7329,7 +7330,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" s="28" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
+      <c r="A14" s="54"/>
       <c r="B14" s="28" t="s">
         <v>74</v>
       </c>
@@ -7362,7 +7363,7 @@
       <c r="K14" s="30"/>
     </row>
     <row r="15" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="51" t="s">
         <v>61</v>
       </c>
       <c r="B15" s="25" t="s">
@@ -7410,7 +7411,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="25" t="s">
         <v>63</v>
       </c>
@@ -7456,7 +7457,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="25" t="s">
         <v>65</v>
       </c>
@@ -7502,7 +7503,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" s="22" customFormat="1" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="52" t="s">
         <v>48</v>
       </c>
       <c r="B18" s="22" t="s">
@@ -7547,7 +7548,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" s="22" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="46"/>
+      <c r="A19" s="52"/>
       <c r="B19" s="22" t="s">
         <v>46</v>
       </c>
@@ -7573,7 +7574,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" s="22" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
+      <c r="A20" s="52"/>
       <c r="B20" s="22" t="s">
         <v>79</v>
       </c>
@@ -7649,7 +7650,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" s="25" customFormat="1" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="51" t="s">
         <v>72</v>
       </c>
       <c r="B22" s="25" t="s">
@@ -7697,7 +7698,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="45"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="25" t="s">
         <v>76</v>
       </c>
@@ -7743,7 +7744,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" s="25" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="45"/>
+      <c r="A24" s="51"/>
       <c r="B24" s="25" t="s">
         <v>77</v>
       </c>
@@ -7787,7 +7788,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" s="22" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="52" t="s">
         <v>78</v>
       </c>
       <c r="B25" s="22" t="s">
@@ -7835,7 +7836,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="46"/>
+      <c r="A26" s="52"/>
       <c r="B26" s="22" t="s">
         <v>79</v>
       </c>
@@ -7852,7 +7853,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" s="22" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="46"/>
+      <c r="A27" s="52"/>
       <c r="B27" s="22" t="s">
         <v>82</v>
       </c>
@@ -7914,7 +7915,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="A1:N28"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7978,7 +7979,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="51" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -8026,7 +8027,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" s="25" customFormat="1" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="25" t="s">
         <v>32</v>
       </c>
@@ -8072,7 +8073,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" s="25" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="25" t="s">
         <v>45</v>
       </c>
@@ -8116,7 +8117,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" s="20" customFormat="1" ht="52" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="53" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="20" t="s">
@@ -8149,7 +8150,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="47"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="20" t="s">
         <v>49</v>
       </c>
@@ -8178,7 +8179,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="47"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="20" t="s">
         <v>50</v>
       </c>
@@ -8207,7 +8208,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" s="20" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="47"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="20" t="s">
         <v>51</v>
       </c>
@@ -8238,7 +8239,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" s="20" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="47"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="20" t="s">
         <v>87</v>
       </c>
@@ -8300,7 +8301,7 @@
       <c r="N10" s="18"/>
     </row>
     <row r="11" spans="1:14" s="28" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="55" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="28" t="s">
@@ -8348,7 +8349,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" s="28" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
+      <c r="A12" s="56"/>
       <c r="B12" s="28" t="s">
         <v>59</v>
       </c>
@@ -8392,7 +8393,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" s="28" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
+      <c r="A13" s="57"/>
       <c r="B13" s="28" t="s">
         <v>74</v>
       </c>
@@ -8425,7 +8426,7 @@
       <c r="K13" s="30"/>
     </row>
     <row r="14" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="51" t="s">
         <v>61</v>
       </c>
       <c r="B14" s="25" t="s">
@@ -8473,7 +8474,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="25" t="s">
         <v>94</v>
       </c>
@@ -8519,7 +8520,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="25" t="s">
         <v>96</v>
       </c>
@@ -8565,7 +8566,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" s="22" customFormat="1" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="52" t="s">
         <v>48</v>
       </c>
       <c r="B17" s="22" t="s">
@@ -8610,7 +8611,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" s="22" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="46"/>
+      <c r="A18" s="52"/>
       <c r="B18" s="22" t="s">
         <v>46</v>
       </c>
@@ -8636,7 +8637,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" s="22" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="46"/>
+      <c r="A19" s="52"/>
       <c r="B19" s="22" t="s">
         <v>79</v>
       </c>
@@ -8667,7 +8668,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" s="41" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="52" t="s">
+      <c r="A20" s="58" t="s">
         <v>71</v>
       </c>
       <c r="B20" s="41" t="s">
@@ -8715,7 +8716,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" s="41" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="52"/>
+      <c r="A21" s="58"/>
       <c r="B21" s="41" t="s">
         <v>30</v>
       </c>
@@ -8758,7 +8759,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="51" t="s">
         <v>72</v>
       </c>
       <c r="B22" s="25" t="s">
@@ -8806,7 +8807,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="45"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="25" t="s">
         <v>103</v>
       </c>
@@ -8852,7 +8853,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="45"/>
+      <c r="A24" s="51"/>
       <c r="B24" s="25" t="s">
         <v>76</v>
       </c>
@@ -8898,7 +8899,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" s="22" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="52" t="s">
         <v>78</v>
       </c>
       <c r="B25" s="22" t="s">
@@ -8946,7 +8947,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="46"/>
+      <c r="A26" s="52"/>
       <c r="B26" s="22" t="s">
         <v>79</v>
       </c>
@@ -8963,7 +8964,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" s="22" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="46"/>
+      <c r="A27" s="52"/>
       <c r="B27" s="22" t="s">
         <v>82</v>
       </c>
@@ -9025,8 +9026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D4E03C-F4BA-7E4B-8E9F-3FB6882BE27A}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:N29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9090,7 +9091,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="51" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -9109,7 +9110,7 @@
         <v>41</v>
       </c>
       <c r="G2" s="27">
-        <f t="shared" ref="G2:G21" si="0">IF(OR(K2="",E2=""),"",K2*E2)</f>
+        <f t="shared" ref="G2:G22" si="0">IF(OR(K2="",E2=""),"",K2*E2)</f>
         <v>136</v>
       </c>
       <c r="H2" s="27">
@@ -9138,7 +9139,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" s="25" customFormat="1" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="25" t="s">
         <v>32</v>
       </c>
@@ -9184,7 +9185,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" s="25" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="25" t="s">
         <v>45</v>
       </c>
@@ -9228,7 +9229,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" s="20" customFormat="1" ht="52" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="53" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="20" t="s">
@@ -9261,7 +9262,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="47"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="20" t="s">
         <v>49</v>
       </c>
@@ -9290,7 +9291,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="47"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="20" t="s">
         <v>50</v>
       </c>
@@ -9319,7 +9320,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" s="20" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="47"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="20" t="s">
         <v>51</v>
       </c>
@@ -9350,7 +9351,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" s="20" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="47"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="20" t="s">
         <v>87</v>
       </c>
@@ -9412,7 +9413,7 @@
       <c r="N10" s="18"/>
     </row>
     <row r="11" spans="1:14" s="28" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="54" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="28" t="s">
@@ -9458,7 +9459,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" s="28" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
+      <c r="A12" s="54"/>
       <c r="B12" s="28" t="s">
         <v>59</v>
       </c>
@@ -9502,7 +9503,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" s="28" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="48"/>
+      <c r="A13" s="54"/>
       <c r="B13" s="28" t="s">
         <v>74</v>
       </c>
@@ -9535,7 +9536,7 @@
       <c r="K13" s="30"/>
     </row>
     <row r="14" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="51" t="s">
         <v>61</v>
       </c>
       <c r="B14" s="25" t="s">
@@ -9583,7 +9584,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="25" t="s">
         <v>94</v>
       </c>
@@ -9629,7 +9630,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="25" t="s">
         <v>105</v>
       </c>
@@ -9675,7 +9676,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="25" t="s">
         <v>98</v>
       </c>
@@ -9721,7 +9722,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" s="22" customFormat="1" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="52" t="s">
         <v>48</v>
       </c>
       <c r="B18" s="22" t="s">
@@ -9769,7 +9770,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" s="22" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="46"/>
+      <c r="A19" s="52"/>
       <c r="B19" s="22" t="s">
         <v>46</v>
       </c>
@@ -9795,7 +9796,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" s="22" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
+      <c r="A20" s="52"/>
       <c r="B20" s="22" t="s">
         <v>79</v>
       </c>
@@ -9826,7 +9827,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" s="41" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53" t="s">
+      <c r="A21" s="59" t="s">
         <v>71</v>
       </c>
       <c r="B21" s="41" t="s">
@@ -9871,7 +9872,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" s="41" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="54"/>
+      <c r="A22" s="60"/>
       <c r="B22" s="41" t="s">
         <v>99</v>
       </c>
@@ -9888,6 +9889,7 @@
         <v>44</v>
       </c>
       <c r="G22" s="41">
+        <f t="shared" si="0"/>
         <v>94</v>
       </c>
       <c r="H22" s="41">
@@ -9913,7 +9915,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" s="25" customFormat="1" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="51" t="s">
         <v>72</v>
       </c>
       <c r="B23" s="25" t="s">
@@ -9961,7 +9963,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="45"/>
+      <c r="A24" s="51"/>
       <c r="B24" s="25" t="s">
         <v>76</v>
       </c>
@@ -10007,7 +10009,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" s="25" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="45"/>
+      <c r="A25" s="51"/>
       <c r="B25" s="25" t="s">
         <v>77</v>
       </c>
@@ -10051,7 +10053,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" s="22" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="46" t="s">
+      <c r="A26" s="52" t="s">
         <v>78</v>
       </c>
       <c r="B26" s="22" t="s">
@@ -10099,7 +10101,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="46"/>
+      <c r="A27" s="52"/>
       <c r="B27" s="22" t="s">
         <v>79</v>
       </c>
@@ -10116,7 +10118,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" s="22" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="46"/>
+      <c r="A28" s="52"/>
       <c r="B28" s="22" t="s">
         <v>82</v>
       </c>
@@ -10179,7 +10181,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView zoomScale="133" workbookViewId="0">
-      <selection activeCell="V32" sqref="A1:XFD1048576"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10243,7 +10245,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="61" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -10291,7 +10293,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67"/>
+      <c r="A3" s="62"/>
       <c r="B3" s="25" t="s">
         <v>30</v>
       </c>
@@ -10337,7 +10339,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" s="25" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="66"/>
+      <c r="A4" s="63"/>
       <c r="B4" s="25" t="s">
         <v>45</v>
       </c>
@@ -10381,7 +10383,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" s="20" customFormat="1" ht="52" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="53" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="20" t="s">
@@ -10414,7 +10416,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="47"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="20" t="s">
         <v>49</v>
       </c>
@@ -10443,7 +10445,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="47"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="20" t="s">
         <v>50</v>
       </c>
@@ -10472,7 +10474,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" s="20" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="47"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="20" t="s">
         <v>51</v>
       </c>
@@ -10503,7 +10505,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" s="20" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="47"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="20" t="s">
         <v>87</v>
       </c>
@@ -10565,7 +10567,7 @@
       <c r="N10" s="18"/>
     </row>
     <row r="11" spans="1:14" s="28" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="55" t="s">
         <v>71</v>
       </c>
       <c r="B11" s="28" t="s">
@@ -10611,7 +10613,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" s="28" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
+      <c r="A12" s="56"/>
       <c r="B12" s="28" t="s">
         <v>59</v>
       </c>
@@ -10655,7 +10657,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" s="28" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
+      <c r="A13" s="57"/>
       <c r="B13" s="28" t="s">
         <v>74</v>
       </c>
@@ -10688,7 +10690,7 @@
       <c r="K13" s="30"/>
     </row>
     <row r="14" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="51" t="s">
         <v>61</v>
       </c>
       <c r="B14" s="25" t="s">
@@ -10736,7 +10738,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="25" t="s">
         <v>112</v>
       </c>
@@ -10782,7 +10784,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="25" t="s">
         <v>98</v>
       </c>
@@ -10828,7 +10830,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="25" t="s">
         <v>94</v>
       </c>
@@ -10874,7 +10876,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" s="22" customFormat="1" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="52" t="s">
         <v>48</v>
       </c>
       <c r="B18" s="22" t="s">
@@ -10919,7 +10921,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" s="22" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="46"/>
+      <c r="A19" s="52"/>
       <c r="B19" s="22" t="s">
         <v>46</v>
       </c>
@@ -10945,7 +10947,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" s="22" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
+      <c r="A20" s="52"/>
       <c r="B20" s="22" t="s">
         <v>79</v>
       </c>
@@ -10976,7 +10978,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" s="41" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="52" t="s">
+      <c r="A21" s="58" t="s">
         <v>71</v>
       </c>
       <c r="B21" s="41" t="s">
@@ -11024,7 +11026,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" s="41" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
+      <c r="A22" s="58"/>
       <c r="B22" s="41" t="s">
         <v>98</v>
       </c>
@@ -11041,7 +11043,8 @@
         <v>44</v>
       </c>
       <c r="G22" s="41">
-        <v>288</v>
+        <f t="shared" si="0"/>
+        <v>192</v>
       </c>
       <c r="H22" s="41">
         <v>63</v>
@@ -11066,7 +11069,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" s="41" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="52"/>
+      <c r="A23" s="58"/>
       <c r="B23" s="28" t="s">
         <v>59</v>
       </c>
@@ -11110,7 +11113,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="45" t="s">
+      <c r="A24" s="51" t="s">
         <v>72</v>
       </c>
       <c r="B24" s="25" t="s">
@@ -11158,7 +11161,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="45"/>
+      <c r="A25" s="51"/>
       <c r="B25" s="25" t="s">
         <v>63</v>
       </c>
@@ -11169,26 +11172,26 @@
         <v>15</v>
       </c>
       <c r="E25" s="33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F25" s="25" t="s">
         <v>44</v>
       </c>
       <c r="G25" s="27">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="H25" s="27">
         <f t="shared" si="1"/>
-        <v>13.2</v>
+        <v>26.4</v>
       </c>
       <c r="I25" s="27">
         <f t="shared" si="2"/>
-        <v>5.6</v>
+        <v>11.2</v>
       </c>
       <c r="J25" s="27">
         <f t="shared" si="3"/>
-        <v>0.8</v>
+        <v>1.6</v>
       </c>
       <c r="K25" s="25">
         <v>34</v>
@@ -11204,7 +11207,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="45"/>
+      <c r="A26" s="51"/>
       <c r="B26" s="25" t="s">
         <v>105</v>
       </c>
@@ -11250,7 +11253,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" s="22" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="52" t="s">
         <v>78</v>
       </c>
       <c r="B27" s="22" t="s">
@@ -11298,7 +11301,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="46"/>
+      <c r="A28" s="52"/>
       <c r="B28" s="22" t="s">
         <v>79</v>
       </c>
@@ -11315,7 +11318,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" s="22" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="46"/>
+      <c r="A29" s="52"/>
       <c r="B29" s="22" t="s">
         <v>82</v>
       </c>
@@ -11342,19 +11345,19 @@
       <c r="E30" s="39"/>
       <c r="G30" s="16">
         <f>SUM(G2:G29)</f>
-        <v>2270</v>
+        <v>2242</v>
       </c>
       <c r="H30" s="16">
         <f>SUM(H2:H29)</f>
-        <v>261.75</v>
+        <v>274.95</v>
       </c>
       <c r="I30" s="16">
         <f>SUM(I2:I29)</f>
-        <v>203.85</v>
+        <v>209.45</v>
       </c>
       <c r="J30" s="16">
         <f>SUM(J2:J29)</f>
-        <v>60.11</v>
+        <v>60.910000000000004</v>
       </c>
       <c r="K30" s="16"/>
     </row>
@@ -11442,7 +11445,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="51" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -11490,7 +11493,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" s="25" customFormat="1" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="25" t="s">
         <v>32</v>
       </c>
@@ -11536,7 +11539,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" s="25" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="25" t="s">
         <v>45</v>
       </c>
@@ -11580,7 +11583,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" s="20" customFormat="1" ht="52" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="53" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="20" t="s">
@@ -11613,7 +11616,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="47"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="20" t="s">
         <v>49</v>
       </c>
@@ -11642,7 +11645,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="47"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="20" t="s">
         <v>50</v>
       </c>
@@ -11671,7 +11674,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" s="20" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="47"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="20" t="s">
         <v>51</v>
       </c>
@@ -11702,7 +11705,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" s="20" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="47"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="20" t="s">
         <v>87</v>
       </c>
@@ -11764,7 +11767,7 @@
       <c r="N10" s="18"/>
     </row>
     <row r="11" spans="1:14" s="28" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="54" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="41" t="s">
@@ -11812,7 +11815,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" s="28" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
+      <c r="A12" s="54"/>
       <c r="B12" s="28" t="s">
         <v>59</v>
       </c>
@@ -11856,7 +11859,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" s="28" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="48"/>
+      <c r="A13" s="54"/>
       <c r="B13" s="28" t="s">
         <v>74</v>
       </c>
@@ -11889,7 +11892,7 @@
       <c r="K13" s="30"/>
     </row>
     <row r="14" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="51" t="s">
         <v>61</v>
       </c>
       <c r="B14" s="25" t="s">
@@ -11937,7 +11940,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="25" t="s">
         <v>94</v>
       </c>
@@ -11983,7 +11986,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="25" t="s">
         <v>105</v>
       </c>
@@ -12029,7 +12032,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="25" t="s">
         <v>96</v>
       </c>
@@ -12075,7 +12078,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" s="22" customFormat="1" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="52" t="s">
         <v>48</v>
       </c>
       <c r="B18" s="22" t="s">
@@ -12120,7 +12123,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" s="22" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="46"/>
+      <c r="A19" s="52"/>
       <c r="B19" s="22" t="s">
         <v>46</v>
       </c>
@@ -12146,7 +12149,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" s="22" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
+      <c r="A20" s="52"/>
       <c r="B20" s="22" t="s">
         <v>79</v>
       </c>
@@ -12177,7 +12180,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" s="41" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53" t="s">
+      <c r="A21" s="59" t="s">
         <v>71</v>
       </c>
       <c r="B21" s="41" t="s">
@@ -12222,7 +12225,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" s="41" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="55"/>
+      <c r="A22" s="64"/>
       <c r="B22" s="41" t="s">
         <v>99</v>
       </c>
@@ -12268,7 +12271,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" s="41" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="54"/>
+      <c r="A23" s="60"/>
       <c r="B23" s="41" t="s">
         <v>30</v>
       </c>
@@ -12314,7 +12317,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" s="25" customFormat="1" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="45" t="s">
+      <c r="A24" s="51" t="s">
         <v>72</v>
       </c>
       <c r="B24" s="25" t="s">
@@ -12362,7 +12365,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="45"/>
+      <c r="A25" s="51"/>
       <c r="B25" s="25" t="s">
         <v>76</v>
       </c>
@@ -12408,7 +12411,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" s="25" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="45"/>
+      <c r="A26" s="51"/>
       <c r="B26" s="25" t="s">
         <v>77</v>
       </c>
@@ -12452,7 +12455,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" s="22" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="52" t="s">
         <v>78</v>
       </c>
       <c r="B27" s="22" t="s">
@@ -12500,7 +12503,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="46"/>
+      <c r="A28" s="52"/>
       <c r="B28" s="22" t="s">
         <v>79</v>
       </c>
@@ -12517,7 +12520,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" s="22" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="46"/>
+      <c r="A29" s="52"/>
       <c r="B29" s="22" t="s">
         <v>82</v>
       </c>
@@ -12580,7 +12583,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="A1:N30"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12644,7 +12647,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="51" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -12692,7 +12695,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" s="25" customFormat="1" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="25" t="s">
         <v>32</v>
       </c>
@@ -12738,7 +12741,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" s="25" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="25" t="s">
         <v>45</v>
       </c>
@@ -12782,7 +12785,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" s="20" customFormat="1" ht="52" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="53" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="20" t="s">
@@ -12815,7 +12818,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="47"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="20" t="s">
         <v>49</v>
       </c>
@@ -12844,7 +12847,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="47"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="20" t="s">
         <v>50</v>
       </c>
@@ -12873,7 +12876,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" s="20" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="47"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="20" t="s">
         <v>51</v>
       </c>
@@ -12904,7 +12907,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" s="20" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="47"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="20" t="s">
         <v>87</v>
       </c>
@@ -12966,7 +12969,7 @@
       <c r="N10" s="18"/>
     </row>
     <row r="11" spans="1:14" s="28" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="55" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="41" t="s">
@@ -13014,7 +13017,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" s="28" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
+      <c r="A12" s="56"/>
       <c r="B12" s="28" t="s">
         <v>59</v>
       </c>
@@ -13058,7 +13061,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" s="28" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
+      <c r="A13" s="57"/>
       <c r="B13" s="28" t="s">
         <v>74</v>
       </c>
@@ -13091,7 +13094,7 @@
       <c r="K13" s="30"/>
     </row>
     <row r="14" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="51" t="s">
         <v>61</v>
       </c>
       <c r="B14" s="25" t="s">
@@ -13139,7 +13142,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="25" t="s">
         <v>94</v>
       </c>
@@ -13185,7 +13188,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="25" t="s">
         <v>98</v>
       </c>
@@ -13231,7 +13234,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" s="22" customFormat="1" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="52" t="s">
         <v>48</v>
       </c>
       <c r="B17" s="22" t="s">
@@ -13276,7 +13279,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" s="22" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="46"/>
+      <c r="A18" s="52"/>
       <c r="B18" s="22" t="s">
         <v>46</v>
       </c>
@@ -13302,7 +13305,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" s="22" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="46"/>
+      <c r="A19" s="52"/>
       <c r="B19" s="22" t="s">
         <v>79</v>
       </c>
@@ -13333,7 +13336,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" s="22" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="65" t="s">
         <v>71</v>
       </c>
       <c r="B20" s="28" t="s">
@@ -13350,19 +13353,19 @@
         <v>60</v>
       </c>
       <c r="G20" s="30">
-        <f t="shared" ref="G20:G21" si="8">IF(OR(K20="",E20=""),"",K20*E20)</f>
+        <f t="shared" ref="G20" si="8">IF(OR(K20="",E20=""),"",K20*E20)</f>
         <v>120</v>
       </c>
       <c r="H20" s="30">
-        <f t="shared" ref="H20:H21" si="9">IF(OR(L20="",E20=""),"",L20*E20)</f>
+        <f t="shared" ref="H20" si="9">IF(OR(L20="",E20=""),"",L20*E20)</f>
         <v>2</v>
       </c>
       <c r="I20" s="30">
-        <f t="shared" ref="I20:I21" si="10">IF(OR(M20="",E20=""),"",M20*E20)</f>
+        <f t="shared" ref="I20" si="10">IF(OR(M20="",E20=""),"",M20*E20)</f>
         <v>24</v>
       </c>
       <c r="J20" s="30">
-        <f t="shared" ref="J20:J21" si="11">IF(OR(N20="",E20=""),"",N20*E20)</f>
+        <f t="shared" ref="J20" si="11">IF(OR(N20="",E20=""),"",N20*E20)</f>
         <v>2</v>
       </c>
       <c r="K20" s="30">
@@ -13379,7 +13382,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" s="41" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="57"/>
+      <c r="A21" s="66"/>
       <c r="B21" s="41" t="s">
         <v>105</v>
       </c>
@@ -13425,7 +13428,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" s="41" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="58"/>
+      <c r="A22" s="67"/>
       <c r="B22" s="41" t="s">
         <v>30</v>
       </c>
@@ -13468,7 +13471,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="51" t="s">
         <v>72</v>
       </c>
       <c r="B23" s="25" t="s">
@@ -13516,7 +13519,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" s="25" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="45"/>
+      <c r="A24" s="51"/>
       <c r="B24" s="25" t="s">
         <v>99</v>
       </c>
@@ -13562,7 +13565,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" s="25" customFormat="1" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="45"/>
+      <c r="A25" s="51"/>
       <c r="B25" s="25" t="s">
         <v>76</v>
       </c>
@@ -13608,7 +13611,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" s="25" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="45"/>
+      <c r="A26" s="51"/>
       <c r="B26" s="25" t="s">
         <v>77</v>
       </c>
@@ -13652,7 +13655,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" s="22" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="52" t="s">
         <v>78</v>
       </c>
       <c r="B27" s="22" t="s">
@@ -13700,7 +13703,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="46"/>
+      <c r="A28" s="52"/>
       <c r="B28" s="22" t="s">
         <v>79</v>
       </c>
@@ -13717,7 +13720,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" s="22" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="46"/>
+      <c r="A29" s="52"/>
       <c r="B29" s="22" t="s">
         <v>82</v>
       </c>

</xml_diff>